<commit_message>
BATRU to BATRU-SAND copy
</commit_message>
<xml_diff>
--- a/Projects/BATRU_SAND/Data/P3_template.xlsx
+++ b/Projects/BATRU_SAND/Data/P3_template.xlsx
@@ -47857,13 +47857,13 @@
   <dimension ref="A1:I278"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4412955465587"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0202429149798"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8097165991903"/>

</xml_diff>

<commit_message>
BATRU to BATRU_SAND copy
</commit_message>
<xml_diff>
--- a/Projects/BATRU_SAND/Data/P3_template.xlsx
+++ b/Projects/BATRU_SAND/Data/P3_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sections" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,6 +49,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
@@ -75,6 +76,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
@@ -101,6 +103,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
@@ -127,6 +130,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
@@ -153,6 +157,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
@@ -179,6 +184,7 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -190,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8940" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8940" uniqueCount="410">
   <si>
     <t xml:space="preserve">State</t>
   </si>
@@ -1290,9 +1296,6 @@
     <t xml:space="preserve">end_shelf</t>
   </si>
   <si>
-    <t xml:space="preserve">pos-000001</t>
-  </si>
-  <si>
     <t xml:space="preserve">product_english_name</t>
   </si>
   <si>
@@ -2013,22 +2016,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8947368421053"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3967611336032"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.753036437247"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3603238866397"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.9068825910931"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.0161943319838"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.9311740890688"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.0364372469636"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.0931174089069"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.9068825910931"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.5465587044534"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.4048582995951"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.2793522267206"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.5668016194332"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47856,19 +47859,19 @@
   </sheetPr>
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A254" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F272" activeCellId="0" sqref="F272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2631578947368"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4412955465587"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8097165991903"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.7125506072874"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="33.1336032388664"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54856,20 +54859,20 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.7651821862348"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3198380566802"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9716599190283"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.67206477732794"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.91902834008097"/>
-    <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.67206477732794"/>
-    <col collapsed="false" hidden="false" max="1025" min="101" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.1295546558704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4"/>
+    <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="1025" min="101" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56106,13 +56109,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.3967611336032"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1821862348178"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8744939271255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8097165991903"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -58386,18 +58389,18 @@
   </sheetPr>
   <dimension ref="A1:C65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B86" activeCellId="0" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="52.7651821862348"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="3.67206477732794"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2388663967611"/>
-    <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.67206477732794"/>
-    <col collapsed="false" hidden="false" max="1025" min="101" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="55.1295546558704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="1025" min="101" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59076,7 +59079,7 @@
         <v>233</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>366</v>
+        <v>234</v>
       </c>
       <c r="C62" s="24" t="n">
         <v>90</v>
@@ -59484,17 +59487,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.18218623481781"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.8056680161943"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="68.919028340081"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.8461538461539"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2793522267206"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C2" s="44" t="s">
         <v>163</v>
@@ -59502,7 +59505,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="45" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C3" s="45" t="s">
         <v>278</v>
@@ -59550,10 +59553,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="45" t="s">
+        <v>368</v>
+      </c>
+      <c r="C9" s="45" t="s">
         <v>369</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59585,7 +59588,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59657,15 +59660,15 @@
         <v>169</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="45" t="s">
+        <v>372</v>
+      </c>
+      <c r="C23" s="45" t="s">
         <v>373</v>
-      </c>
-      <c r="C23" s="45" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59742,10 +59745,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="45" t="s">
+        <v>374</v>
+      </c>
+      <c r="C33" s="45" t="s">
         <v>375</v>
-      </c>
-      <c r="C33" s="45" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59785,7 +59788,7 @@
         <v>353</v>
       </c>
       <c r="C38" s="45" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59818,7 +59821,7 @@
     </row>
     <row r="43" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C43" s="45"/>
     </row>
@@ -59828,10 +59831,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="45" t="s">
+        <v>378</v>
+      </c>
+      <c r="C45" s="45" t="s">
         <v>379</v>
-      </c>
-      <c r="C45" s="45" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59887,7 +59890,7 @@
         <v>288</v>
       </c>
       <c r="C52" s="46" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60031,7 +60034,7 @@
         <v>323</v>
       </c>
       <c r="C70" s="45" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60055,7 +60058,7 @@
         <v>326</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60071,7 +60074,7 @@
         <v>335</v>
       </c>
       <c r="C75" s="45" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60087,7 +60090,7 @@
         <v>336</v>
       </c>
       <c r="C77" s="45" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60103,7 +60106,7 @@
         <v>347</v>
       </c>
       <c r="C79" s="47" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -60132,12 +60135,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4817813765182"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.7692307692308"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.8987854251012"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="110.303643724696"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.1336032388664"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="66.8421052631579"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="115.400809716599"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60145,16 +60148,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>387</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="52" t="s">
         <v>388</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="E1" s="53" t="s">
         <v>389</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60168,10 +60171,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60185,10 +60188,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60202,10 +60205,10 @@
         <v>46</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60219,10 +60222,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60236,10 +60239,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60253,10 +60256,10 @@
         <v>46</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60270,10 +60273,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60287,10 +60290,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>399</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60304,10 +60307,10 @@
         <v>46</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60321,10 +60324,10 @@
         <v>46</v>
       </c>
       <c r="D11" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>403</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60338,10 +60341,10 @@
         <v>46</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60355,10 +60358,10 @@
         <v>16</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60372,10 +60375,10 @@
         <v>16</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>399</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60389,10 +60392,10 @@
         <v>46</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60406,10 +60409,10 @@
         <v>46</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>403</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60423,10 +60426,10 @@
         <v>46</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60440,10 +60443,10 @@
         <v>16</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60457,10 +60460,10 @@
         <v>16</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60474,10 +60477,10 @@
         <v>46</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60491,10 +60494,10 @@
         <v>16</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60508,10 +60511,10 @@
         <v>16</v>
       </c>
       <c r="D22" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60525,10 +60528,10 @@
         <v>46</v>
       </c>
       <c r="D23" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60542,10 +60545,10 @@
         <v>16</v>
       </c>
       <c r="D24" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60559,10 +60562,10 @@
         <v>16</v>
       </c>
       <c r="D25" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>407</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60576,10 +60579,10 @@
         <v>46</v>
       </c>
       <c r="D26" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60593,10 +60596,10 @@
         <v>46</v>
       </c>
       <c r="D27" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>409</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60610,10 +60613,10 @@
         <v>46</v>
       </c>
       <c r="D28" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60627,10 +60630,10 @@
         <v>16</v>
       </c>
       <c r="D29" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60644,10 +60647,10 @@
         <v>16</v>
       </c>
       <c r="D30" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>407</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60661,10 +60664,10 @@
         <v>46</v>
       </c>
       <c r="D31" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60678,10 +60681,10 @@
         <v>46</v>
       </c>
       <c r="D32" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>409</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60695,10 +60698,10 @@
         <v>46</v>
       </c>
       <c r="D33" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60712,10 +60715,10 @@
         <v>16</v>
       </c>
       <c r="D34" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60729,10 +60732,10 @@
         <v>16</v>
       </c>
       <c r="D35" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60746,10 +60749,10 @@
         <v>46</v>
       </c>
       <c r="D36" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60763,10 +60766,10 @@
         <v>16</v>
       </c>
       <c r="D37" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60780,10 +60783,10 @@
         <v>16</v>
       </c>
       <c r="D38" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60797,10 +60800,10 @@
         <v>46</v>
       </c>
       <c r="D39" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60814,10 +60817,10 @@
         <v>16</v>
       </c>
       <c r="D40" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60831,10 +60834,10 @@
         <v>16</v>
       </c>
       <c r="D41" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>407</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60848,10 +60851,10 @@
         <v>46</v>
       </c>
       <c r="D42" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60865,10 +60868,10 @@
         <v>46</v>
       </c>
       <c r="D43" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>409</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60882,10 +60885,10 @@
         <v>46</v>
       </c>
       <c r="D44" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60899,10 +60902,10 @@
         <v>16</v>
       </c>
       <c r="D45" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60916,10 +60919,10 @@
         <v>16</v>
       </c>
       <c r="D46" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>407</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60933,10 +60936,10 @@
         <v>46</v>
       </c>
       <c r="D47" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60950,10 +60953,10 @@
         <v>46</v>
       </c>
       <c r="D48" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="E48" s="0" t="s">
         <v>409</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60967,10 +60970,10 @@
         <v>46</v>
       </c>
       <c r="D49" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E49" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>